<commit_message>
Small fixes + new obosolete names
</commit_message>
<xml_diff>
--- a/genus_descriptions/genus_descriptions.xlsx
+++ b/genus_descriptions/genus_descriptions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>genus</t>
   </si>
@@ -25,6 +25,9 @@
     <t>properties</t>
   </si>
   <si>
+    <t>references</t>
+  </si>
+  <si>
     <t>Lactobacillus</t>
   </si>
   <si>
@@ -103,7 +106,7 @@
     <t>Lactobacilli from fields</t>
   </si>
   <si>
-    <t xml:space="preserve"> A. composti</t>
+    <t>A. composti</t>
   </si>
   <si>
     <t>Homofermentative, aerotolerant and vancomycin resistant. Genome size, G+C content of the genome and the source of the two species suggest a free-living lifestyle of the genus.</t>
@@ -145,16 +148,16 @@
     <t>Homofermentative, vancomycin resistant; many species ferment pentoses, and are resistant to oxidative stress. L. casei and related species have a nomadic lifestyle.</t>
   </si>
   <si>
-    <t>Latilactobacillus,</t>
+    <t>Latilactobacillus</t>
   </si>
   <si>
     <t>Wide-spread lactobacilli</t>
   </si>
   <si>
-    <t xml:space="preserve"> L. sakei</t>
-  </si>
-  <si>
-    <t>Homofermentative, mesophilic free living and environmental lactobacilli. Many strains are psychrotrophic and grow below 8 °C.</t>
+    <t>L. sakei</t>
+  </si>
+  <si>
+    <t>Homofermentative, vancomycin resistant, mesophilic free living and environmental lactobacilli. Many strains are psychrotrophic and grow below 8 °C.</t>
   </si>
   <si>
     <t>Dellaglioa</t>
@@ -181,6 +184,9 @@
     <t>Homofermentative, vancomycin resistant, motile organisms growing in liquid, plant-associated habitats. Many liquorilactobacilli produce EPS from sucrose and degrade fructans with extracellular fructanases.</t>
   </si>
   <si>
+    <t>10.1021/acs.jafc.0c02313</t>
+  </si>
+  <si>
     <t>Ligilactobacillus</t>
   </si>
   <si>
@@ -203,6 +209,10 @@
   </si>
   <si>
     <t>Homofermentative, vancomycin resistant organisms with a nomadic lifestyle that ferment a wide range of carbohydrates; most species metabolise phenolic acids by esterase, decarboxylase and reductase activities. Lactiplantibacillus plantarum expresses pseudocatalase and nitrate reductase activities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1186/1475-2859-10-S1-S3, 10.1016/S0969-2126(01)00628-1, 10.1128/AEM.00147-09, 10.1111/1462-2920.13455, 10.1016/B978-0-12-802309-9.00004-2, 10.1128/AEM.02461-19, 10.1016/j.syapm.2004.11.004.
+      </t>
   </si>
   <si>
     <t>Furfurilactobacillus</t>
@@ -317,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -326,6 +336,36 @@
     <font>
       <b/>
       <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -333,16 +373,7 @@
       <sz val="8.0"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="8.0"/>
-      <name val="Arial"/>
-    </font>
     <font/>
-    <font>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -377,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -387,19 +418,31 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -631,351 +674,360 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="D5" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="D8" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="D9" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="7" t="s">
         <v>39</v>
       </c>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="7" t="s">
         <v>43</v>
       </c>
+      <c r="D11" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="8" t="s">
         <v>47</v>
       </c>
+      <c r="D12" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="7" t="s">
         <v>51</v>
       </c>
+      <c r="D13" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>55</v>
       </c>
+      <c r="D14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="C15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="C16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="B17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>75</v>
       </c>
+      <c r="B19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="B20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>83</v>
       </c>
+      <c r="B21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>87</v>
       </c>
+      <c r="B22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="B23" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="B24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="B25" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="7"/>
+      <c r="A26" s="11"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add newly described taxa
</commit_message>
<xml_diff>
--- a/genus_descriptions/genus_descriptions.xlsx
+++ b/genus_descriptions/genus_descriptions.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuyts\Documents\Projects\new_lactobacillus_taxonomy\lactotax\genus_descriptions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0A0192-23A3-467C-B433-CB1C6D955098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="27525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -320,64 +329,74 @@
     <t>L. buchneri</t>
   </si>
   <si>
-    <t>Heterofermentative, vancomycin resistant, mesophilic, fermenting a broad spectrum of carbohydrates. Few lentilactobacilli appear to transition to a host-adapted lifestyle but most are environmental or plant-associated. Most lentilactobacilli metabolise agmatine and convert lactate and / or diols.</t>
+    <t xml:space="preserve">Heterofermentative, vancomycin resistant, mesophilic, fermenting a broad spectrum of carbohydrates. Most lentilactobacilli are environmental or plant-associated, metabolise agmatine and convert lactate and / or diols. L. senioris and L. kribbianus form an outgroup to the genus; both species were isolated from vertrebrates and may transition to a host-adapted lifestyle. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
-      <sz val="8.0"/>
-      <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
-      <sz val="11.0"/>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -385,11 +404,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -403,62 +428,61 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -648,26 +672,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.14"/>
-    <col customWidth="1" min="2" max="2" width="78.71"/>
-    <col customWidth="1" min="3" max="3" width="14.0"/>
-    <col customWidth="1" min="4" max="4" width="220.71"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="78.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="220.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -698,7 +727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -712,7 +741,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -726,7 +755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -740,7 +769,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -754,7 +783,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
@@ -768,7 +797,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -782,7 +811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -796,7 +825,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
@@ -810,7 +839,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
@@ -824,7 +853,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>45</v>
       </c>
@@ -838,7 +867,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>49</v>
       </c>
@@ -852,7 +881,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
@@ -869,7 +898,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>58</v>
       </c>
@@ -883,7 +912,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>62</v>
       </c>
@@ -900,7 +929,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>67</v>
       </c>
@@ -914,7 +943,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>71</v>
       </c>
@@ -928,7 +957,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>75</v>
       </c>
@@ -942,7 +971,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>79</v>
       </c>
@@ -956,7 +985,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>83</v>
       </c>
@@ -970,7 +999,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>87</v>
       </c>
@@ -984,7 +1013,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>91</v>
       </c>
@@ -998,7 +1027,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>95</v>
       </c>
@@ -1012,7 +1041,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>99</v>
       </c>
@@ -1022,14 +1051,15 @@
       <c r="C25" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add genus description for new genera
</commit_message>
<xml_diff>
--- a/genus_descriptions/genus_descriptions.xlsx
+++ b/genus_descriptions/genus_descriptions.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuyts\Documents\Projects\new_lactobacillus_taxonomy\lactotax\genus_descriptions\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0A0192-23A3-467C-B433-CB1C6D955098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="27525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>genus</t>
   </si>
@@ -49,7 +40,7 @@
     <t>Homofermentative with strain-specific ability to ferment pentoses, thermophilic, vancomycin-sensitive, adapted to vertebrate or insect hosts.</t>
   </si>
   <si>
-    <t>Holzapfelia</t>
+    <t>Holzapfeliella</t>
   </si>
   <si>
     <t>Wilhelm Holzapfel’s lactobacilli</t>
@@ -155,6 +146,18 @@
   </si>
   <si>
     <t>Homofermentative, vancomycin resistant; many species ferment pentoses, and are resistant to oxidative stress. L. casei and related species have a nomadic lifestyle.</t>
+  </si>
+  <si>
+    <t>Paralactobacillus</t>
+  </si>
+  <si>
+    <t>closely related to lactobacilli</t>
+  </si>
+  <si>
+    <t>P. selangorensis</t>
+  </si>
+  <si>
+    <t>Homofermentative, vancomycin resistant, mesophilic organism.</t>
   </si>
   <si>
     <t>Latilactobacillus</t>
@@ -254,7 +257,7 @@
     <t>Slimy (biofilm-forming) lactobacilli</t>
   </si>
   <si>
-    <t>L. fermentum</t>
+    <t>L  fermentum</t>
   </si>
   <si>
     <t>Heterofermentative, thermophilic, vancomycin resistant with two exceptions, Limosilactobacillus species are vertebrate host adapted and generally form exopolysaccharides from sucrose to support biofilm formation in the upper intestine of animals.</t>
@@ -282,6 +285,33 @@
   </si>
   <si>
     <t>Heterofermentative, vancomycin resistant, grow in the pH range of 3 – 5; fermenting disaccharides and sugar alcohols but few hexoses and no pentoses.</t>
+  </si>
+  <si>
+    <t>Philodulcilactobacillus</t>
+  </si>
+  <si>
+    <t>Sugar-loving lactobacilli</t>
+  </si>
+  <si>
+    <t>Pl. myokoensis</t>
+  </si>
+  <si>
+    <t>Heterofermentative, vancomycin resistant, fructiphlic, growth on media solidified with gellan gum but not with agar</t>
+  </si>
+  <si>
+    <t>Nicoliella</t>
+  </si>
+  <si>
+    <t>Nicola Spurrier’s lactobacilli</t>
+  </si>
+  <si>
+    <t>N. spurrieriana</t>
+  </si>
+  <si>
+    <t>Heterofermentative, vancomycin resistant, small genome size but the single Nicoliella species has a broader carbohydrate fermentation pattern and a larger genome size than the closely related apilactobacilli. Likely adapted to bees or flowers.</t>
+  </si>
+  <si>
+    <t>10.1099/ijsem.0.005588</t>
   </si>
   <si>
     <t>Apilactobacillus</t>
@@ -335,68 +365,63 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="8"/>
+      <sz val="8.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
+      <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <i/>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="&quot;Calibri&quot;"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="&quot;Calibri&quot;"/>
+    </font>
+    <font>
+      <i/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
-      <sz val="8"/>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Arial&quot;"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="&quot;Calibri&quot;"/>
     </font>
   </fonts>
   <fills count="2">
@@ -404,17 +429,11 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -428,61 +447,71 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -672,66 +701,61 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="220.7109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="14.13"/>
+    <col customWidth="1" min="2" max="2" width="68.88"/>
+    <col customWidth="1" min="3" max="3" width="12.25"/>
+    <col customWidth="1" min="4" max="4" width="193.13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -741,11 +765,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -755,11 +779,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -769,11 +793,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -783,11 +807,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7">
+      <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -797,11 +821,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8">
+      <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -811,25 +835,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9">
+      <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="10">
+      <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -839,11 +863,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="11">
+      <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -853,39 +877,39 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    <row r="12">
+      <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="13">
+      <c r="A13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14">
+      <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -894,29 +918,29 @@
       <c r="D14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="3" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="16">
+      <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -925,29 +949,29 @@
       <c r="D16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="10" t="s">
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18">
+      <c r="A18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -957,11 +981,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19">
+      <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -971,11 +995,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="20">
+      <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -985,11 +1009,11 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="21">
+      <c r="A21" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -999,67 +1023,111 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22">
+      <c r="A22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23">
+      <c r="A23" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="9" t="s">
         <v>92</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="24">
+      <c r="A24" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="13" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="5" t="s">
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
+      <c r="D25" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="14"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>